<commit_message>
Auto-install dependencies in start.bat
</commit_message>
<xml_diff>
--- a/backend/uploads/JJMMTT___MUBEA_BEISPIEL_BOM_KIPOC_abgespeckt.xlsx
+++ b/backend/uploads/JJMMTT___MUBEA_BEISPIEL_BOM_KIPOC_abgespeckt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr updateLinks="always" hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csientw.sharepoint.com/sites/iCSIIPAICommunityTeams-DrawingAI/Shared Documents/Drawing AI/Test-Daten/Stüli fuer Test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkp.CSI\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{F83EEC6E-1020-4835-B12F-A860A3529973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BBEE37D-A7A8-4D3E-BED9-821FEDD98B66}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9364B8-413E-4ABB-A1A5-A9C06B5F74EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4F777920-6EF3-48A4-862C-8FA1D9AA837F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{4F777920-6EF3-48A4-862C-8FA1D9AA837F}"/>
   </bookViews>
   <sheets>
     <sheet name="V1.0" sheetId="29" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3282" uniqueCount="1431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3290" uniqueCount="1433">
   <si>
     <t>-</t>
   </si>
@@ -4392,6 +4392,12 @@
   </si>
   <si>
     <t>Bauteilbenennung</t>
+  </si>
+  <si>
+    <t>002_005_105_01</t>
+  </si>
+  <si>
+    <t>111_222_333_00</t>
   </si>
 </sst>
 </file>
@@ -6115,6 +6121,24 @@
     <xf numFmtId="14" fontId="0" fillId="22" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6184,24 +6208,6 @@
     <xf numFmtId="49" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6262,7 +6268,17 @@
     <cellStyle name="Standard 9" xfId="13" xr:uid="{64481A11-0225-4167-9E4D-F99BB23D4D25}"/>
     <cellStyle name="Währung 2" xfId="4" xr:uid="{C6DDC917-228F-495A-845D-9755B55041EC}"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -6465,7 +6481,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle13" displayName="Tabelle13" ref="B2:B9" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle13" displayName="Tabelle13" ref="B2:B9" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="B2:B9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Freigabestand"/>
@@ -6475,7 +6491,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabelle134" displayName="Tabelle134" ref="D2:D51" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabelle134" displayName="Tabelle134" ref="D2:D51" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="D2:D51" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Werkstoff"/>
@@ -6485,7 +6501,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabelle135" displayName="Tabelle135" ref="F2:F19" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tabelle135" displayName="Tabelle135" ref="F2:F19" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="F2:F19" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Beschichtung"/>
@@ -6495,7 +6511,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabelle136" displayName="Tabelle136" ref="H2:H21" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabelle136" displayName="Tabelle136" ref="H2:H21" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="H2:H21" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Fertigungsverfahren"/>
@@ -6805,31 +6821,31 @@
     <outlinePr summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BD44"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" customHeight="1" outlineLevelCol="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15" customHeight="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="91.42578125" customWidth="1" outlineLevel="2"/>
-    <col min="2" max="2" width="20.28515625" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="29.28515625" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="76.7109375" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="6.5703125" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="7.42578125" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="8.85546875" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="7.5703125" customWidth="1" outlineLevel="1"/>
+    <col min="1" max="1" width="91.44140625" customWidth="1" outlineLevel="2"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="4" max="4" width="5.44140625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="29.33203125" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="76.6640625" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="6.5546875" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="7.44140625" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="8.88671875" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="7.5546875" customWidth="1" outlineLevel="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="101.25" thickBot="1">
+    <row r="1" spans="1:13" ht="94.2" thickBot="1">
       <c r="A1" s="140" t="s">
         <v>1429</v>
       </c>
@@ -6870,55 +6886,55 @@
     </row>
     <row r="2" spans="1:13" s="83" customFormat="1" ht="15" customHeight="1" thickBot="1">
       <c r="A2" s="197" t="str">
-        <f>A1</f>
+        <f t="shared" ref="A2:M2" si="0">A1</f>
         <v>Bauteilbenennung CAD</v>
       </c>
       <c r="B2" s="197" t="str">
-        <f>B1</f>
+        <f t="shared" si="0"/>
         <v>Bauteil</v>
       </c>
       <c r="C2" s="197" t="str">
-        <f>C1</f>
+        <f t="shared" si="0"/>
         <v>Teilenummer</v>
       </c>
       <c r="D2" s="197" t="str">
-        <f>D1</f>
+        <f t="shared" si="0"/>
         <v>Version/Revisonsnr.</v>
       </c>
       <c r="E2" s="198" t="str">
-        <f>E1</f>
+        <f t="shared" si="0"/>
         <v>Bauteilbenennung</v>
       </c>
       <c r="F2" s="198">
-        <f>F1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G2" s="197" t="str">
-        <f>G1</f>
+        <f t="shared" si="0"/>
         <v>Werkstoff</v>
       </c>
       <c r="H2" s="197" t="str">
-        <f>H1</f>
+        <f t="shared" si="0"/>
         <v>Beschichtung</v>
       </c>
       <c r="I2" s="197" t="str">
-        <f>I1</f>
+        <f t="shared" si="0"/>
         <v>Dichte</v>
       </c>
       <c r="J2" s="197" t="str">
-        <f>J1</f>
+        <f t="shared" si="0"/>
         <v>Material-stärke</v>
       </c>
       <c r="K2" s="197" t="str">
-        <f>K1</f>
+        <f t="shared" si="0"/>
         <v>Anzahl</v>
       </c>
       <c r="L2" s="197" t="str">
-        <f>L1</f>
+        <f t="shared" si="0"/>
         <v>Gewicht</v>
       </c>
       <c r="M2" s="197" t="str">
-        <f>M1</f>
+        <f t="shared" si="0"/>
         <v>∑</v>
       </c>
     </row>
@@ -6926,20 +6942,19 @@
       <c r="A3" s="175" t="s">
         <v>1428</v>
       </c>
-      <c r="B3" s="173" t="str">
-        <f>(C3&amp;"_"&amp;D3)</f>
-        <v>111_222_333_00</v>
+      <c r="B3" s="200" t="s">
+        <v>1432</v>
       </c>
       <c r="C3" s="173" t="str">
-        <f>LEFT(A3,11)</f>
+        <f t="shared" ref="C3:C10" si="1">LEFT(A3,11)</f>
         <v>111_222_333</v>
       </c>
       <c r="D3" s="196" t="str">
-        <f>MID(A3,13,2)</f>
+        <f t="shared" ref="D3:D10" si="2">MID(A3,13,2)</f>
         <v>00</v>
       </c>
       <c r="E3" s="125" t="str">
-        <f>MID(A3,28,FIND("__",A3)-28)</f>
+        <f t="shared" ref="E3:E10" si="3">MID(A3,28,FIND("__",A3)-28)</f>
         <v>TESTPRODUCT</v>
       </c>
       <c r="F3" s="125"/>
@@ -6969,20 +6984,19 @@
       <c r="A4" s="199" t="s">
         <v>1407</v>
       </c>
-      <c r="B4" s="200" t="str">
-        <f>(C4&amp;"_"&amp;D4)</f>
-        <v>002_005_105_01</v>
+      <c r="B4" s="200" t="s">
+        <v>1431</v>
       </c>
       <c r="C4" s="200" t="str">
-        <f>LEFT(A4,11)</f>
+        <f t="shared" si="1"/>
         <v>002_005_105</v>
       </c>
       <c r="D4" s="201" t="str">
-        <f>MID(A4,13,2)</f>
+        <f t="shared" si="2"/>
         <v>01</v>
       </c>
       <c r="E4" s="202" t="str">
-        <f>MID(A4,28,FIND("__",A4)-28)</f>
+        <f t="shared" si="3"/>
         <v>SPACER_AH_1</v>
       </c>
       <c r="F4" s="203"/>
@@ -7005,7 +7019,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="M4" s="179">
-        <f>K4*L4</f>
+        <f t="shared" ref="M4:M10" si="4">K4*L4</f>
         <v>8.3000000000000004E-2</v>
       </c>
     </row>
@@ -7013,20 +7027,19 @@
       <c r="A5" s="137" t="s">
         <v>1422</v>
       </c>
-      <c r="B5" s="138" t="str">
-        <f>(C5&amp;"_"&amp;D5)</f>
-        <v>111_222_333_00</v>
+      <c r="B5" s="138" t="s">
+        <v>1432</v>
       </c>
       <c r="C5" s="138" t="str">
-        <f>LEFT(A5,11)</f>
+        <f t="shared" si="1"/>
         <v>111_222_333</v>
       </c>
       <c r="D5" s="105" t="str">
-        <f>MID(A5,13,2)</f>
+        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="E5" s="134" t="str">
-        <f>MID(A5,28,FIND("__",A5)-28)</f>
+        <f t="shared" si="3"/>
         <v>ALU_PROFIL</v>
       </c>
       <c r="F5" s="135"/>
@@ -7049,7 +7062,7 @@
         <v>0.02</v>
       </c>
       <c r="M5" s="126">
-        <f>K5*L5</f>
+        <f t="shared" si="4"/>
         <v>0.02</v>
       </c>
     </row>
@@ -7057,20 +7070,19 @@
       <c r="A6" s="137" t="s">
         <v>1423</v>
       </c>
-      <c r="B6" s="138" t="str">
-        <f>(C6&amp;"_"&amp;D6)</f>
-        <v>111_222_333_00</v>
+      <c r="B6" s="138" t="s">
+        <v>1432</v>
       </c>
       <c r="C6" s="138" t="str">
-        <f>LEFT(A6,11)</f>
+        <f t="shared" si="1"/>
         <v>111_222_333</v>
       </c>
       <c r="D6" s="105" t="str">
-        <f>MID(A6,13,2)</f>
+        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="E6" s="134" t="str">
-        <f>MID(A6,28,FIND("__",A6)-28)</f>
+        <f t="shared" si="3"/>
         <v>BLECH</v>
       </c>
       <c r="F6" s="135"/>
@@ -7093,7 +7105,7 @@
         <v>0.41199999999999998</v>
       </c>
       <c r="M6" s="126">
-        <f>K6*L6</f>
+        <f t="shared" si="4"/>
         <v>0.82399999999999995</v>
       </c>
     </row>
@@ -7101,20 +7113,19 @@
       <c r="A7" s="106" t="s">
         <v>1424</v>
       </c>
-      <c r="B7" s="133" t="str">
-        <f>(C7&amp;"_"&amp;D7)</f>
-        <v>111_222_333_00</v>
+      <c r="B7" s="133" t="s">
+        <v>1432</v>
       </c>
       <c r="C7" s="133" t="str">
-        <f>LEFT(A7,11)</f>
+        <f t="shared" si="1"/>
         <v>111_222_333</v>
       </c>
       <c r="D7" s="174" t="str">
-        <f>MID(A7,13,2)</f>
+        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="E7" s="29" t="str">
-        <f>MID(A7,28,FIND("__",A7)-28)</f>
+        <f t="shared" si="3"/>
         <v>DREHTEIL</v>
       </c>
       <c r="F7" s="32"/>
@@ -7137,7 +7148,7 @@
         <v>3.8090000000000002</v>
       </c>
       <c r="M7" s="123">
-        <f>K7*L7</f>
+        <f t="shared" si="4"/>
         <v>19.045000000000002</v>
       </c>
     </row>
@@ -7145,20 +7156,19 @@
       <c r="A8" s="109" t="s">
         <v>1425</v>
       </c>
-      <c r="B8" s="112" t="str">
-        <f>(C8&amp;"_"&amp;D8)</f>
-        <v>111_222_333_00</v>
+      <c r="B8" s="112" t="s">
+        <v>1432</v>
       </c>
       <c r="C8" s="112" t="str">
-        <f>LEFT(A8,11)</f>
+        <f t="shared" si="1"/>
         <v>111_222_333</v>
       </c>
       <c r="D8" s="130" t="str">
-        <f>MID(A8,13,2)</f>
+        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="E8" s="104" t="str">
-        <f>MID(A8,28,FIND("__",A8)-28)</f>
+        <f t="shared" si="3"/>
         <v>GUSSTEIL</v>
       </c>
       <c r="F8" s="124"/>
@@ -7181,7 +7191,7 @@
         <v>0.28799999999999998</v>
       </c>
       <c r="M8" s="207">
-        <f>K8*L8</f>
+        <f t="shared" si="4"/>
         <v>0.28799999999999998</v>
       </c>
     </row>
@@ -7189,20 +7199,19 @@
       <c r="A9" s="106" t="s">
         <v>1426</v>
       </c>
-      <c r="B9" s="133" t="str">
-        <f>(C9&amp;"_"&amp;D9)</f>
-        <v>111_222_333_00</v>
+      <c r="B9" s="133" t="s">
+        <v>1432</v>
       </c>
       <c r="C9" s="133" t="str">
-        <f>LEFT(A9,11)</f>
+        <f t="shared" si="1"/>
         <v>111_222_333</v>
       </c>
       <c r="D9" s="174" t="str">
-        <f>MID(A9,13,2)</f>
+        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="E9" s="29" t="str">
-        <f>MID(A9,28,FIND("__",A9)-28)</f>
+        <f t="shared" si="3"/>
         <v>KUNSTSTOFF</v>
       </c>
       <c r="F9" s="32"/>
@@ -7225,7 +7234,7 @@
         <v>0.16300000000000001</v>
       </c>
       <c r="M9" s="123">
-        <f>K9*L9</f>
+        <f t="shared" si="4"/>
         <v>0.16300000000000001</v>
       </c>
     </row>
@@ -7233,20 +7242,19 @@
       <c r="A10" s="109" t="s">
         <v>1427</v>
       </c>
-      <c r="B10" s="112" t="str">
-        <f>(C10&amp;"_"&amp;D10)</f>
-        <v>111_222_333_00</v>
+      <c r="B10" s="112" t="s">
+        <v>1432</v>
       </c>
       <c r="C10" s="112" t="str">
-        <f>LEFT(A10,11)</f>
+        <f t="shared" si="1"/>
         <v>111_222_333</v>
       </c>
       <c r="D10" s="130" t="str">
-        <f>MID(A10,13,2)</f>
+        <f t="shared" si="2"/>
         <v>00</v>
       </c>
       <c r="E10" s="104" t="str">
-        <f>MID(A10,28,FIND("__",A10)-28)</f>
+        <f t="shared" si="3"/>
         <v>STAHL_PROFIL</v>
       </c>
       <c r="F10" s="124"/>
@@ -7269,7 +7277,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="M10" s="207">
-        <f>K10*L10</f>
+        <f t="shared" si="4"/>
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
@@ -7300,7 +7308,7 @@
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <conditionalFormatting sqref="B3:B10">
-    <cfRule type="duplicateValues" dxfId="1" priority="15981"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="15982"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="12" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -7313,41 +7321,41 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:35">
@@ -7793,141 +7801,141 @@
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.5703125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.5546875" style="16" customWidth="1"/>
     <col min="3" max="3" width="13" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="9" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.5703125" style="16" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="17" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" style="49" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" style="49" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.5546875" style="16" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.44140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.44140625" style="17" customWidth="1"/>
+    <col min="11" max="11" width="18.5546875" style="49" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" style="49" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="24" style="16" customWidth="1"/>
     <col min="14" max="14" width="17" style="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.42578125" style="40" customWidth="1"/>
+    <col min="15" max="15" width="20.44140625" style="40" customWidth="1"/>
     <col min="16" max="16" width="14" style="9" customWidth="1"/>
-    <col min="17" max="17" width="255.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="255.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5546875" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="224" t="s">
+      <c r="A1" s="230" t="s">
         <v>373</v>
       </c>
-      <c r="B1" s="225"/>
-      <c r="C1" s="225"/>
-      <c r="D1" s="225"/>
-      <c r="E1" s="225"/>
-      <c r="F1" s="225"/>
-      <c r="G1" s="225"/>
-      <c r="H1" s="225"/>
-      <c r="I1" s="225"/>
-      <c r="J1" s="225"/>
-      <c r="K1" s="225"/>
-      <c r="L1" s="225"/>
-      <c r="M1" s="225"/>
-      <c r="N1" s="225"/>
-      <c r="O1" s="225"/>
-      <c r="P1" s="225"/>
-      <c r="Q1" s="225"/>
-      <c r="R1" s="226"/>
+      <c r="B1" s="231"/>
+      <c r="C1" s="231"/>
+      <c r="D1" s="231"/>
+      <c r="E1" s="231"/>
+      <c r="F1" s="231"/>
+      <c r="G1" s="231"/>
+      <c r="H1" s="231"/>
+      <c r="I1" s="231"/>
+      <c r="J1" s="231"/>
+      <c r="K1" s="231"/>
+      <c r="L1" s="231"/>
+      <c r="M1" s="231"/>
+      <c r="N1" s="231"/>
+      <c r="O1" s="231"/>
+      <c r="P1" s="231"/>
+      <c r="Q1" s="231"/>
+      <c r="R1" s="232"/>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1">
-      <c r="A2" s="227"/>
-      <c r="B2" s="232"/>
-      <c r="C2" s="232" t="s">
+      <c r="A2" s="233"/>
+      <c r="B2" s="238"/>
+      <c r="C2" s="238" t="s">
         <v>374</v>
       </c>
-      <c r="D2" s="221" t="s">
+      <c r="D2" s="227" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="221" t="s">
+      <c r="E2" s="227" t="s">
         <v>375</v>
       </c>
-      <c r="F2" s="233" t="s">
+      <c r="F2" s="239" t="s">
         <v>358</v>
       </c>
-      <c r="G2" s="234" t="s">
+      <c r="G2" s="240" t="s">
         <v>376</v>
       </c>
-      <c r="H2" s="235" t="s">
+      <c r="H2" s="241" t="s">
         <v>377</v>
       </c>
-      <c r="I2" s="235" t="s">
+      <c r="I2" s="241" t="s">
         <v>378</v>
       </c>
-      <c r="J2" s="236" t="s">
+      <c r="J2" s="242" t="s">
         <v>379</v>
       </c>
-      <c r="K2" s="244" t="s">
+      <c r="K2" s="221" t="s">
         <v>380</v>
       </c>
       <c r="L2" s="59"/>
-      <c r="M2" s="241" t="s">
+      <c r="M2" s="218" t="s">
         <v>76</v>
       </c>
-      <c r="N2" s="234" t="s">
+      <c r="N2" s="240" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="238" t="s">
+      <c r="O2" s="244" t="s">
         <v>381</v>
       </c>
       <c r="P2" s="90"/>
-      <c r="Q2" s="218" t="s">
+      <c r="Q2" s="224" t="s">
         <v>382</v>
       </c>
-      <c r="R2" s="237" t="s">
+      <c r="R2" s="243" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1">
-      <c r="A3" s="228"/>
-      <c r="B3" s="232"/>
-      <c r="C3" s="232"/>
-      <c r="D3" s="222"/>
-      <c r="E3" s="230"/>
-      <c r="F3" s="233"/>
-      <c r="G3" s="234"/>
-      <c r="H3" s="235"/>
-      <c r="I3" s="235"/>
-      <c r="J3" s="236"/>
-      <c r="K3" s="245"/>
+      <c r="A3" s="234"/>
+      <c r="B3" s="238"/>
+      <c r="C3" s="238"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="236"/>
+      <c r="F3" s="239"/>
+      <c r="G3" s="240"/>
+      <c r="H3" s="241"/>
+      <c r="I3" s="241"/>
+      <c r="J3" s="242"/>
+      <c r="K3" s="222"/>
       <c r="L3" s="60" t="s">
         <v>383</v>
       </c>
-      <c r="M3" s="242"/>
-      <c r="N3" s="234"/>
-      <c r="O3" s="239"/>
+      <c r="M3" s="219"/>
+      <c r="N3" s="240"/>
+      <c r="O3" s="245"/>
       <c r="P3" s="91" t="s">
         <v>384</v>
       </c>
-      <c r="Q3" s="219"/>
-      <c r="R3" s="237"/>
+      <c r="Q3" s="225"/>
+      <c r="R3" s="243"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1">
-      <c r="A4" s="229"/>
-      <c r="B4" s="232"/>
-      <c r="C4" s="232"/>
-      <c r="D4" s="223"/>
-      <c r="E4" s="231"/>
-      <c r="F4" s="233"/>
-      <c r="G4" s="234"/>
-      <c r="H4" s="235"/>
-      <c r="I4" s="235"/>
-      <c r="J4" s="236"/>
-      <c r="K4" s="246"/>
+      <c r="A4" s="235"/>
+      <c r="B4" s="238"/>
+      <c r="C4" s="238"/>
+      <c r="D4" s="229"/>
+      <c r="E4" s="237"/>
+      <c r="F4" s="239"/>
+      <c r="G4" s="240"/>
+      <c r="H4" s="241"/>
+      <c r="I4" s="241"/>
+      <c r="J4" s="242"/>
+      <c r="K4" s="223"/>
       <c r="L4" s="61"/>
-      <c r="M4" s="243"/>
-      <c r="N4" s="234"/>
-      <c r="O4" s="240"/>
+      <c r="M4" s="220"/>
+      <c r="N4" s="240"/>
+      <c r="O4" s="246"/>
       <c r="P4" s="92"/>
-      <c r="Q4" s="220"/>
-      <c r="R4" s="237"/>
+      <c r="Q4" s="226"/>
+      <c r="R4" s="243"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1">
       <c r="B5" s="38"/>
@@ -14869,7 +14877,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:17" ht="16.5">
+    <row r="143" spans="1:17" ht="16.8">
       <c r="A143" s="16">
         <v>138</v>
       </c>
@@ -20787,6 +20795,8 @@
   </sheetData>
   <autoFilter ref="A5:R288" xr:uid="{F3C867EE-EFC6-47C2-A5CB-79FA4F40CE33}"/>
   <mergeCells count="17">
+    <mergeCell ref="O2:O4"/>
+    <mergeCell ref="M2:M4"/>
     <mergeCell ref="K2:K4"/>
     <mergeCell ref="Q2:Q4"/>
     <mergeCell ref="D2:D4"/>
@@ -20802,8 +20812,6 @@
     <mergeCell ref="J2:J4"/>
     <mergeCell ref="N2:N4"/>
     <mergeCell ref="R2:R4"/>
-    <mergeCell ref="O2:O4"/>
-    <mergeCell ref="M2:M4"/>
   </mergeCells>
   <phoneticPr fontId="17" type="noConversion"/>
   <hyperlinks>
@@ -20904,17 +20912,17 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="22.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="33.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" customWidth="1"/>
-    <col min="4" max="4" width="93.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="83.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="40.5703125" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" customWidth="1"/>
+    <col min="4" max="4" width="93.44140625" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
+    <col min="6" max="6" width="83.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="40.5546875" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" customWidth="1"/>
+    <col min="10" max="10" width="7.5546875" customWidth="1"/>
     <col min="11" max="11" width="111" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -20964,7 +20972,7 @@
       <c r="U2" s="252"/>
       <c r="V2" s="253"/>
     </row>
-    <row r="3" spans="2:22" ht="15.75" thickBot="1">
+    <row r="3" spans="2:22" ht="15" thickBot="1">
       <c r="B3" s="33" t="s">
         <v>110</v>
       </c>
@@ -20998,7 +21006,7 @@
       <c r="U3" s="118"/>
       <c r="V3" s="119"/>
     </row>
-    <row r="4" spans="2:22" ht="16.5" thickTop="1" thickBot="1">
+    <row r="4" spans="2:22" ht="15.6" thickTop="1" thickBot="1">
       <c r="B4" t="s">
         <v>1267</v>
       </c>
@@ -21042,7 +21050,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="5" spans="2:22" ht="15.75" thickBot="1">
+    <row r="5" spans="2:22" ht="15" thickBot="1">
       <c r="B5" t="s">
         <v>337</v>
       </c>
@@ -21086,7 +21094,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="6" spans="2:22" ht="15.75" thickBot="1">
+    <row r="6" spans="2:22" ht="15" thickBot="1">
       <c r="B6" t="s">
         <v>99</v>
       </c>
@@ -21130,7 +21138,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="7" spans="2:22" ht="15.75" thickBot="1">
+    <row r="7" spans="2:22" ht="15" thickBot="1">
       <c r="B7" t="s">
         <v>84</v>
       </c>
@@ -21172,7 +21180,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="8" spans="2:22" ht="15.75" thickBot="1">
+    <row r="8" spans="2:22" ht="15" thickBot="1">
       <c r="B8" s="2" t="s">
         <v>168</v>
       </c>
@@ -21216,7 +21224,7 @@
         <v>5.0199999999999996</v>
       </c>
     </row>
-    <row r="9" spans="2:22" ht="15.75" thickBot="1">
+    <row r="9" spans="2:22" ht="15" thickBot="1">
       <c r="B9" t="s">
         <v>297</v>
       </c>
@@ -21257,7 +21265,7 @@
         <v>10.18</v>
       </c>
     </row>
-    <row r="10" spans="2:22" ht="15.75" thickBot="1">
+    <row r="10" spans="2:22" ht="15" thickBot="1">
       <c r="D10" t="s">
         <v>1286</v>
       </c>
@@ -21289,7 +21297,7 @@
         <v>17.29</v>
       </c>
     </row>
-    <row r="11" spans="2:22" ht="15.75" thickBot="1">
+    <row r="11" spans="2:22" ht="15" thickBot="1">
       <c r="D11" t="s">
         <v>236</v>
       </c>
@@ -21321,7 +21329,7 @@
         <v>23.1</v>
       </c>
     </row>
-    <row r="12" spans="2:22" ht="15.75" thickBot="1">
+    <row r="12" spans="2:22" ht="15" thickBot="1">
       <c r="D12" t="s">
         <v>240</v>
       </c>
@@ -21353,7 +21361,7 @@
         <v>42.07</v>
       </c>
     </row>
-    <row r="13" spans="2:22" ht="15.75" thickBot="1">
+    <row r="13" spans="2:22" ht="15" thickBot="1">
       <c r="D13" t="s">
         <v>1292</v>
       </c>
@@ -21385,7 +21393,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="2:22" ht="15.75" thickBot="1">
+    <row r="14" spans="2:22" ht="15" thickBot="1">
       <c r="D14" t="s">
         <v>1294</v>
       </c>
@@ -21417,7 +21425,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="2:22" ht="15.75" thickBot="1">
+    <row r="15" spans="2:22" ht="15" thickBot="1">
       <c r="D15" t="s">
         <v>1295</v>
       </c>
@@ -21449,7 +21457,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="16" spans="2:22" ht="15.75" thickBot="1">
+    <row r="16" spans="2:22" ht="15" thickBot="1">
       <c r="D16" t="s">
         <v>124</v>
       </c>
@@ -21481,7 +21489,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="17" spans="4:22" ht="15.75" thickBot="1">
+    <row r="17" spans="4:22" ht="15" thickBot="1">
       <c r="D17" t="s">
         <v>1301</v>
       </c>
@@ -21513,7 +21521,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="18" spans="4:22" ht="15.75" thickBot="1">
+    <row r="18" spans="4:22" ht="15" thickBot="1">
       <c r="D18" t="s">
         <v>115</v>
       </c>
@@ -21545,7 +21553,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="19" spans="4:22" ht="15.75" thickBot="1">
+    <row r="19" spans="4:22" ht="15" thickBot="1">
       <c r="D19" t="s">
         <v>1308</v>
       </c>
@@ -21577,7 +21585,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="20" spans="4:22" ht="15.75" thickBot="1">
+    <row r="20" spans="4:22" ht="15" thickBot="1">
       <c r="D20" t="s">
         <v>117</v>
       </c>
@@ -21606,7 +21614,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="21" spans="4:22" ht="15.75" thickBot="1">
+    <row r="21" spans="4:22" ht="15" thickBot="1">
       <c r="D21" t="s">
         <v>173</v>
       </c>
@@ -21635,7 +21643,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="22" spans="4:22" ht="15.75" thickBot="1">
+    <row r="22" spans="4:22" ht="15" thickBot="1">
       <c r="D22" t="s">
         <v>96</v>
       </c>
@@ -21661,7 +21669,7 @@
         <v>2438</v>
       </c>
     </row>
-    <row r="23" spans="4:22" ht="15.75" thickBot="1">
+    <row r="23" spans="4:22" ht="15" thickBot="1">
       <c r="D23" t="s">
         <v>1322</v>
       </c>
@@ -21687,7 +21695,7 @@
         <v>3323</v>
       </c>
     </row>
-    <row r="24" spans="4:22" ht="15.75" thickBot="1">
+    <row r="24" spans="4:22" ht="15" thickBot="1">
       <c r="D24" t="s">
         <v>1325</v>
       </c>
@@ -21713,7 +21721,7 @@
         <v>4266</v>
       </c>
     </row>
-    <row r="25" spans="4:22" ht="15.75" thickBot="1">
+    <row r="25" spans="4:22" ht="15" thickBot="1">
       <c r="D25" t="s">
         <v>1329</v>
       </c>
@@ -21739,7 +21747,7 @@
         <v>5529</v>
       </c>
     </row>
-    <row r="26" spans="4:22" ht="15.75" thickBot="1">
+    <row r="26" spans="4:22" ht="15" thickBot="1">
       <c r="D26" t="s">
         <v>305</v>
       </c>
@@ -21765,7 +21773,7 @@
         <v>6835</v>
       </c>
     </row>
-    <row r="27" spans="4:22" ht="15.75" thickBot="1">
+    <row r="27" spans="4:22" ht="15" thickBot="1">
       <c r="D27" t="s">
         <v>155</v>
       </c>
@@ -21791,7 +21799,7 @@
         <v>8541</v>
       </c>
     </row>
-    <row r="28" spans="4:22" ht="15.75" thickBot="1">
+    <row r="28" spans="4:22" ht="15" thickBot="1">
       <c r="D28" t="s">
         <v>1336</v>
       </c>
@@ -21817,7 +21825,7 @@
         <v>10271</v>
       </c>
     </row>
-    <row r="29" spans="4:22" ht="15.75" thickBot="1">
+    <row r="29" spans="4:22" ht="15" thickBot="1">
       <c r="D29" s="14" t="s">
         <v>183</v>
       </c>
@@ -21843,7 +21851,7 @@
         <v>13292</v>
       </c>
     </row>
-    <row r="30" spans="4:22" ht="15.75" thickBot="1">
+    <row r="30" spans="4:22" ht="15" thickBot="1">
       <c r="D30" t="s">
         <v>1341</v>
       </c>
@@ -21869,7 +21877,7 @@
         <v>16526</v>
       </c>
     </row>
-    <row r="31" spans="4:22" ht="15.75" thickBot="1">
+    <row r="31" spans="4:22" ht="15" thickBot="1">
       <c r="D31" t="s">
         <v>1344</v>
       </c>
@@ -21895,7 +21903,7 @@
         <v>20619</v>
       </c>
     </row>
-    <row r="32" spans="4:22" ht="15.75" thickBot="1">
+    <row r="32" spans="4:22" ht="15" thickBot="1">
       <c r="D32" t="s">
         <v>1347</v>
       </c>
@@ -21921,7 +21929,7 @@
         <v>24911</v>
       </c>
     </row>
-    <row r="33" spans="3:22" ht="15.75" thickBot="1">
+    <row r="33" spans="3:22" ht="15" thickBot="1">
       <c r="D33" t="s">
         <v>1350</v>
       </c>
@@ -21947,7 +21955,7 @@
         <v>1353</v>
       </c>
     </row>
-    <row r="34" spans="3:22" ht="15.75" thickTop="1">
+    <row r="34" spans="3:22" ht="15" thickTop="1">
       <c r="C34" t="s">
         <v>1</v>
       </c>
@@ -22083,14 +22091,14 @@
       <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="11" width="10.42578125" customWidth="1"/>
-    <col min="17" max="17" width="78.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="11" width="10.44140625" customWidth="1"/>
+    <col min="17" max="17" width="78.5546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.44140625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -23629,5 +23637,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8099F7D3-BDE1-4B3B-8F4D-926082C2C9C3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8099F7D3-BDE1-4B3B-8F4D-926082C2C9C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d9079aea-ed8a-47ff-be1f-05d891e7bea7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>